<commit_message>
Working with Futures and Observables to try to reduce the time to find first solve
</commit_message>
<xml_diff>
--- a/Experiment/PuzzleSolveParVsSeqRun.xlsx
+++ b/Experiment/PuzzleSolveParVsSeqRun.xlsx
@@ -9,12 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045" tabRatio="775" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Hardest Puzzle" sheetId="1" r:id="rId1"/>
     <sheet name="Puzzles from websudoku - level1" sheetId="3" r:id="rId2"/>
     <sheet name="Puzzles from websudoku - level4" sheetId="2" r:id="rId3"/>
+    <sheet name="Solve2" sheetId="4" r:id="rId4"/>
+    <sheet name="Solve3" sheetId="5" r:id="rId5"/>
+    <sheet name="Solve4" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
   <si>
     <t>Par</t>
   </si>
@@ -41,6 +44,9 @@
   </si>
   <si>
     <t>Min</t>
+  </si>
+  <si>
+    <t>Async</t>
   </si>
 </sst>
 </file>
@@ -349,11 +355,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="404609184"/>
-        <c:axId val="404609728"/>
+        <c:axId val="1181482608"/>
+        <c:axId val="1181489680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="404609184"/>
+        <c:axId val="1181482608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -413,7 +419,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404609728"/>
+        <c:crossAx val="1181489680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -421,7 +427,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="404609728"/>
+        <c:axId val="1181489680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -536,7 +542,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404609184"/>
+        <c:crossAx val="1181482608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -835,11 +841,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="488989136"/>
-        <c:axId val="488999472"/>
+        <c:axId val="1181490768"/>
+        <c:axId val="1181491312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="488989136"/>
+        <c:axId val="1181490768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -900,7 +906,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="488999472"/>
+        <c:crossAx val="1181491312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -908,7 +914,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="488999472"/>
+        <c:axId val="1181491312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -969,7 +975,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="488989136"/>
+        <c:crossAx val="1181490768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1290,11 +1296,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="541361472"/>
-        <c:axId val="541359840"/>
+        <c:axId val="1181490224"/>
+        <c:axId val="1181483152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="541361472"/>
+        <c:axId val="1181490224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1325,6 +1331,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1354,7 +1361,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="541359840"/>
+        <c:crossAx val="1181483152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1362,7 +1369,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="541359840"/>
+        <c:axId val="1181483152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1423,7 +1430,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="541361472"/>
+        <c:crossAx val="1181490224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1437,7 +1444,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1722,11 +1728,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="541358752"/>
-        <c:axId val="541352768"/>
+        <c:axId val="1181492400"/>
+        <c:axId val="1181481520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="541358752"/>
+        <c:axId val="1181492400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1786,7 +1792,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="541352768"/>
+        <c:crossAx val="1181481520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1794,7 +1800,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="541352768"/>
+        <c:axId val="1181481520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1855,7 +1861,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="541358752"/>
+        <c:crossAx val="1181492400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1869,7 +1875,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4695,7 +4700,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4969,8 +4974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5445,4 +5450,445 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>57719598898</v>
+      </c>
+      <c r="B1">
+        <f>A1/1000000000</f>
+        <v>57.719598898000001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>58023811826</v>
+      </c>
+      <c r="B2">
+        <f>A2/1000000000</f>
+        <v>58.023811825999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>37647574863</v>
+      </c>
+      <c r="B2">
+        <f>A2/1000000000</f>
+        <v>37.647574863000003</v>
+      </c>
+      <c r="D2">
+        <v>84320732746</v>
+      </c>
+      <c r="E2">
+        <f>D2/1000000000</f>
+        <v>84.320732746000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>35351821976</v>
+      </c>
+      <c r="B3">
+        <f>A3/1000000000</f>
+        <v>35.351821975999997</v>
+      </c>
+      <c r="D3">
+        <v>82711369779</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E19" si="0">D3/1000000000</f>
+        <v>82.711369778999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>45335242553</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ref="B5:B21" si="1">A5/1000000000</f>
+        <v>45.335242553</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>43258363231</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="1"/>
+        <v>43.258363230999997</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>42267225511</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>42.267225510999999</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>29921752119</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>29.921752119000001</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>117717162966</v>
+      </c>
+      <c r="B1">
+        <f>A1/1000000000</f>
+        <v>117.717162966</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>82244142373</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="B2:B21" si="0">A2/1000000000</f>
+        <v>82.244142373000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>38497570580</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>38.497570580000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>39724303789</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>39.724303788999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>38246429884</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>38.246429884000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>23403074462</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>23.403074461999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>27738861755</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>27.738861754999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>34065698346</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>34.065698345999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added exp results for method 4 of puzzle solve
</commit_message>
<xml_diff>
--- a/Experiment/PuzzleSolveParVsSeqRun.xlsx
+++ b/Experiment/PuzzleSolveParVsSeqRun.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
   <si>
     <t>Par</t>
   </si>
@@ -47,6 +47,15 @@
   </si>
   <si>
     <t>Async</t>
+  </si>
+  <si>
+    <t>Level 4</t>
+  </si>
+  <si>
+    <t>Level 1</t>
+  </si>
+  <si>
+    <t>Warmup</t>
   </si>
 </sst>
 </file>
@@ -1444,6 +1453,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1875,6 +1885,776 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Solve4!$B$1:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>38.497570580000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39.724303788999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38.246429884000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.403074461999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.738861754999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34.065698345999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28.846853992</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27.278163721999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>28.408414882999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>35.488750537999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1017836320"/>
+        <c:axId val="1017836864"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1017836320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1017836864"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1017836864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1017836320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Solve4!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Level 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Solve4!$H$2:$H$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>3037589394</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1639287323</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2753879197</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1930128476</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2757024080</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2744453624</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1537867881</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2940192735</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1670650107</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1409121860</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1220772259</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2077544851</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1896056204</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1529964817</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1971116964</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1557638373</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2174903220</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4071073504</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2370100749</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Solve4!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Level 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Solve4!$I$2:$I$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>885464574</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>822040318</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>922122384</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>765524779</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>760688835</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>776807597</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>772078627</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>768388215</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1084007909</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>770759805</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>757839216</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>827370476</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>983524393</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>752684322</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>748622855</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>758990275</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>761179495</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>757258160</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>753820380</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1253291392"/>
+        <c:axId val="1253303360"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1253291392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1253303360"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1253303360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1253291392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2103,6 +2883,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
   <cs:axisTitle>
@@ -3751,6 +4611,1058 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4434,6 +6346,71 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5726,169 +7703,445 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>117717162966</v>
+        <v>38497570580</v>
       </c>
       <c r="B1">
         <f>A1/1000000000</f>
-        <v>117.717162966</v>
+        <v>38.497570580000001</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>82244142373</v>
+        <v>39724303789</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:B21" si="0">A2/1000000000</f>
-        <v>82.244142373000003</v>
+        <f>A2/1000000000</f>
+        <v>39.724303788999997</v>
+      </c>
+      <c r="E2">
+        <v>7060335031</v>
+      </c>
+      <c r="F2">
+        <v>2038255712</v>
+      </c>
+      <c r="H2">
+        <v>3037589394</v>
+      </c>
+      <c r="I2">
+        <v>885464574</v>
+      </c>
+      <c r="K2">
+        <f>E2/1000000000</f>
+        <v>7.0603350310000001</v>
+      </c>
+      <c r="L2">
+        <f>F2/1000000000</f>
+        <v>2.0382557120000002</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>38246429884</v>
+      </c>
       <c r="B3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>A3/1000000000</f>
+        <v>38.246429884000001</v>
+      </c>
+      <c r="E3">
+        <v>2052828679</v>
+      </c>
+      <c r="F3">
+        <v>1765751754</v>
+      </c>
+      <c r="H3">
+        <v>1639287323</v>
+      </c>
+      <c r="I3">
+        <v>822040318</v>
+      </c>
+      <c r="K3">
+        <f>E3/1000000000</f>
+        <v>2.0528286790000001</v>
+      </c>
+      <c r="L3">
+        <f>F3/1000000000</f>
+        <v>1.7657517540000001</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>23403074462</v>
+      </c>
       <c r="B4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>A4/1000000000</f>
+        <v>23.403074461999999</v>
+      </c>
+      <c r="H4">
+        <v>2753879197</v>
+      </c>
+      <c r="I4">
+        <v>922122384</v>
+      </c>
+      <c r="K4">
+        <f>H2/1000000000</f>
+        <v>3.0375893939999998</v>
+      </c>
+      <c r="L4">
+        <f>I2/1000000000</f>
+        <v>0.885464574</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>38497570580</v>
+        <v>27738861755</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
-        <v>38.497570580000001</v>
+        <f>A5/1000000000</f>
+        <v>27.738861754999999</v>
+      </c>
+      <c r="H5">
+        <v>1930128476</v>
+      </c>
+      <c r="I5">
+        <v>765524779</v>
+      </c>
+      <c r="K5">
+        <f>H3/1000000000</f>
+        <v>1.639287323</v>
+      </c>
+      <c r="L5">
+        <f>I3/1000000000</f>
+        <v>0.82204031799999999</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>39724303789</v>
+        <v>34065698346</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
-        <v>39.724303788999997</v>
+        <f>A6/1000000000</f>
+        <v>34.065698345999998</v>
+      </c>
+      <c r="H6">
+        <v>2757024080</v>
+      </c>
+      <c r="I6">
+        <v>760688835</v>
+      </c>
+      <c r="K6">
+        <f>H4/1000000000</f>
+        <v>2.7538791969999998</v>
+      </c>
+      <c r="L6">
+        <f>I4/1000000000</f>
+        <v>0.92212238400000002</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>38246429884</v>
+        <v>28846853992</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
-        <v>38.246429884000001</v>
+        <f>A7/1000000000</f>
+        <v>28.846853992</v>
+      </c>
+      <c r="H7">
+        <v>2744453624</v>
+      </c>
+      <c r="I7">
+        <v>776807597</v>
+      </c>
+      <c r="K7">
+        <f>H5/1000000000</f>
+        <v>1.9301284759999999</v>
+      </c>
+      <c r="L7">
+        <f>I5/1000000000</f>
+        <v>0.76552477900000004</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>27278163722</v>
+      </c>
       <c r="B8">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>A8/1000000000</f>
+        <v>27.278163721999999</v>
+      </c>
+      <c r="H8">
+        <v>1537867881</v>
+      </c>
+      <c r="I8">
+        <v>772078627</v>
+      </c>
+      <c r="K8">
+        <f>H6/1000000000</f>
+        <v>2.7570240799999999</v>
+      </c>
+      <c r="L8">
+        <f>I6/1000000000</f>
+        <v>0.76068883499999995</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>23403074462</v>
+        <v>28408414883</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
-        <v>23.403074461999999</v>
+        <f>A9/1000000000</f>
+        <v>28.408414882999999</v>
+      </c>
+      <c r="H9">
+        <v>2940192735</v>
+      </c>
+      <c r="I9">
+        <v>768388215</v>
+      </c>
+      <c r="K9">
+        <f>H7/1000000000</f>
+        <v>2.7444536240000001</v>
+      </c>
+      <c r="L9">
+        <f>I7/1000000000</f>
+        <v>0.77680759700000002</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>27738861755</v>
+        <v>35488750538</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
-        <v>27.738861754999999</v>
+        <f>A10/1000000000</f>
+        <v>35.488750537999998</v>
+      </c>
+      <c r="H10">
+        <v>1670650107</v>
+      </c>
+      <c r="I10">
+        <v>1084007909</v>
+      </c>
+      <c r="K10">
+        <f>H8/1000000000</f>
+        <v>1.5378678809999999</v>
+      </c>
+      <c r="L10">
+        <f>I8/1000000000</f>
+        <v>0.77207862699999996</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>1409121860</v>
+      </c>
+      <c r="I11">
+        <v>770759805</v>
+      </c>
+      <c r="K11">
+        <f>H9/1000000000</f>
+        <v>2.9401927350000001</v>
+      </c>
+      <c r="L11">
+        <f>I9/1000000000</f>
+        <v>0.76838821499999999</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>34065698346</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>34.065698345999998</v>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>1220772259</v>
+      </c>
+      <c r="I12">
+        <v>757839216</v>
+      </c>
+      <c r="K12">
+        <f>H10/1000000000</f>
+        <v>1.6706501069999999</v>
+      </c>
+      <c r="L12">
+        <f>I10/1000000000</f>
+        <v>1.0840079090000001</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>0</v>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <v>2077544851</v>
+      </c>
+      <c r="I13">
+        <v>827370476</v>
+      </c>
+      <c r="K13">
+        <f>H11/1000000000</f>
+        <v>1.4091218599999999</v>
+      </c>
+      <c r="L13">
+        <f>I11/1000000000</f>
+        <v>0.77075980499999996</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>0</v>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>1896056204</v>
+      </c>
+      <c r="I14">
+        <v>983524393</v>
+      </c>
+      <c r="K14">
+        <f>H12/1000000000</f>
+        <v>1.2207722590000001</v>
+      </c>
+      <c r="L14">
+        <f>I12/1000000000</f>
+        <v>0.75783921600000004</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>0</v>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>1529964817</v>
+      </c>
+      <c r="I15">
+        <v>752684322</v>
+      </c>
+      <c r="K15">
+        <f>H13/1000000000</f>
+        <v>2.0775448509999999</v>
+      </c>
+      <c r="L15">
+        <f>I13/1000000000</f>
+        <v>0.82737047600000002</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>0</v>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>1971116964</v>
+      </c>
+      <c r="I16">
+        <v>748622855</v>
+      </c>
+      <c r="K16">
+        <f>H14/1000000000</f>
+        <v>1.896056204</v>
+      </c>
+      <c r="L16">
+        <f>I14/1000000000</f>
+        <v>0.98352439300000005</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>0</v>
+    <row r="17" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>1557638373</v>
+      </c>
+      <c r="I17">
+        <v>758990275</v>
+      </c>
+      <c r="K17">
+        <f>H15/1000000000</f>
+        <v>1.529964817</v>
+      </c>
+      <c r="L17">
+        <f>I15/1000000000</f>
+        <v>0.75268432200000002</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <f t="shared" si="0"/>
-        <v>0</v>
+    <row r="18" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>2174903220</v>
+      </c>
+      <c r="I18">
+        <v>761179495</v>
+      </c>
+      <c r="K18">
+        <f>H16/1000000000</f>
+        <v>1.9711169639999999</v>
+      </c>
+      <c r="L18">
+        <f>I16/1000000000</f>
+        <v>0.74862285500000003</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <f t="shared" si="0"/>
-        <v>0</v>
+    <row r="19" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>4071073504</v>
+      </c>
+      <c r="I19">
+        <v>757258160</v>
+      </c>
+      <c r="K19">
+        <f>H17/1000000000</f>
+        <v>1.5576383730000001</v>
+      </c>
+      <c r="L19">
+        <f>I17/1000000000</f>
+        <v>0.75899027500000005</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>0</v>
+    <row r="20" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>2370100749</v>
+      </c>
+      <c r="I20">
+        <v>753820380</v>
+      </c>
+      <c r="K20">
+        <f>H18/1000000000</f>
+        <v>2.17490322</v>
+      </c>
+      <c r="L20">
+        <f>I18/1000000000</f>
+        <v>0.76117949500000004</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <f t="shared" si="0"/>
-        <v>0</v>
+    <row r="21" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <f>H19/1000000000</f>
+        <v>4.0710735040000001</v>
+      </c>
+      <c r="L21">
+        <f>I19/1000000000</f>
+        <v>0.75725816000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <f>H20/1000000000</f>
+        <v>2.3701007490000001</v>
+      </c>
+      <c r="L22">
+        <f>I20/1000000000</f>
+        <v>0.75382037999999996</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>